<commit_message>
added selection for BeNeRail
</commit_message>
<xml_diff>
--- a/mock/mock scenario variations.xlsx
+++ b/mock/mock scenario variations.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EXG310\Desktop\OSDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB78ACD6-1B75-45E2-806E-E94DE87941D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9013BA3F-10B2-4030-81BC-FC669339A311}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DE5B4741-31D0-4410-9DC9-14C5DAA36404}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Features grid" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="130">
   <si>
     <t>Shopping</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Not represented</t>
-  </si>
-  <si>
-    <t>with included ancillaries</t>
   </si>
   <si>
     <t>with optional ancillaries</t>
@@ -157,9 +154,6 @@
 GET /locations</t>
   </si>
   <si>
-    <t>Get a pass offer</t>
-  </si>
-  <si>
     <t>POST /non-trip-offers-collection</t>
   </si>
   <si>
@@ -401,6 +395,36 @@
   </si>
   <si>
     <t>Renfe</t>
+  </si>
+  <si>
+    <t>with included local transportation in the admission</t>
+  </si>
+  <si>
+    <t>with included ancillaries (could be a separate local transportation travel right)</t>
+  </si>
+  <si>
+    <t>Trenitalia</t>
+  </si>
+  <si>
+    <t>&lt;check trenitalia prez&gt;</t>
+  </si>
+  <si>
+    <t>for top comfort class</t>
+  </si>
+  <si>
+    <t>with "sub-comfort" classes(ex: eurostar business &amp; premier)</t>
+  </si>
+  <si>
+    <t>Get a non-trip offer</t>
+  </si>
+  <si>
+    <t>internal error on provider side</t>
+  </si>
+  <si>
+    <t>fulfilling an already fulfilled tickets</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -416,12 +440,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -436,9 +472,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -459,7 +500,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -755,16 +796,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D972A9-C9B8-47DC-8286-D5354F5EB344}">
-  <dimension ref="A1:O74"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomRight" activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
@@ -783,42 +824,45 @@
     <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
         <v>102</v>
       </c>
-      <c r="F1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>104</v>
       </c>
-      <c r="H1" t="s">
-        <v>106</v>
-      </c>
       <c r="I1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="N1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" t="s">
         <v>118</v>
       </c>
-      <c r="O1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -835,37 +879,40 @@
         <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N2" t="s">
+        <v>117</v>
+      </c>
+      <c r="O2" t="s">
         <v>119</v>
       </c>
-      <c r="O2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -876,10 +923,10 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -887,10 +934,10 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -898,10 +945,10 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -909,10 +956,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -925,421 +972,476 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+      <c r="L20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+      <c r="L29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L36" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" t="s">
+    <row r="43" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+    <row r="44" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
+    <row r="45" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>58</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>59</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
         <v>65</v>
       </c>
-      <c r="B46" t="s">
+      <c r="L51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>66</v>
       </c>
-      <c r="D46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
+      <c r="D56" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>71</v>
+      </c>
+      <c r="L60" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
         <v>81</v>
       </c>
-      <c r="D61" t="s">
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>85</v>
+      </c>
+      <c r="D66" t="s">
+        <v>62</v>
+      </c>
+      <c r="L66" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
+      <c r="D67" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>87</v>
       </c>
-      <c r="D63" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>84</v>
-      </c>
-      <c r="D64" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D65" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="D70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>88</v>
       </c>
-      <c r="D66" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+      <c r="B71" t="s">
         <v>89</v>
       </c>
-      <c r="D67" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="D71" t="s">
         <v>90</v>
       </c>
-      <c r="B68" t="s">
+      <c r="L71" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
         <v>91</v>
       </c>
-      <c r="D68" t="s">
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D69" t="s">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
+      <c r="L76" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="D77" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>98</v>
-      </c>
-      <c r="D74" t="s">
-        <v>99</v>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update from DB for Scenarios
</commit_message>
<xml_diff>
--- a/mock/mock scenario variations.xlsx
+++ b/mock/mock scenario variations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EXG310\Desktop\OSDM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\BKU\ralfrabayer\OSDM\mock\OSDM\mock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9013BA3F-10B2-4030-81BC-FC669339A311}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7834DF-EEDF-4BA3-B351-7074956E80D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DE5B4741-31D0-4410-9DC9-14C5DAA36404}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{DE5B4741-31D0-4410-9DC9-14C5DAA36404}"/>
   </bookViews>
   <sheets>
     <sheet name="Features grid" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="132">
   <si>
     <t>Shopping</t>
   </si>
@@ -425,6 +425,12 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>? - if no one else does this.</t>
   </si>
 </sst>
 </file>
@@ -472,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -482,9 +488,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -500,7 +507,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -799,10 +806,10 @@
   <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L64" sqref="L64"/>
+      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +821,7 @@
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -834,7 +841,7 @@
       <c r="G1" t="s">
         <v>102</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>104</v>
       </c>
       <c r="I1" t="s">
@@ -884,7 +891,7 @@
       <c r="G2" t="s">
         <v>101</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="5" t="s">
         <v>107</v>
       </c>
       <c r="I2" t="s">
@@ -972,6 +979,9 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
+      <c r="H7" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="L7" t="s">
         <v>129</v>
       </c>
@@ -980,6 +990,9 @@
       <c r="D8" t="s">
         <v>24</v>
       </c>
+      <c r="H8" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="L8" t="s">
         <v>129</v>
       </c>
@@ -998,16 +1011,25 @@
       <c r="D11" t="s">
         <v>53</v>
       </c>
+      <c r="H11" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>54</v>
       </c>
+      <c r="H12" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>25</v>
       </c>
+      <c r="H13" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
@@ -1018,6 +1040,9 @@
       <c r="D15" t="s">
         <v>17</v>
       </c>
+      <c r="H15" s="5" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
@@ -1051,11 +1076,17 @@
       <c r="D21" t="s">
         <v>26</v>
       </c>
+      <c r="H21" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>20</v>
       </c>
+      <c r="H22" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
@@ -1081,6 +1112,9 @@
       <c r="D27" t="s">
         <v>41</v>
       </c>
+      <c r="H27" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="28" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
@@ -1109,6 +1143,9 @@
       <c r="D32" t="s">
         <v>120</v>
       </c>
+      <c r="H32" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
@@ -1170,6 +1207,7 @@
       <c r="D40" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="H40" s="5"/>
     </row>
     <row r="41" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
@@ -1181,21 +1219,25 @@
       <c r="D41" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D42" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D43" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="H43" s="5"/>
     </row>
     <row r="44" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D44" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="H44" s="5"/>
     </row>
     <row r="45" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
@@ -1207,6 +1249,7 @@
       <c r="D45" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="H45" s="5"/>
     </row>
     <row r="46" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
@@ -1218,6 +1261,7 @@
       <c r="D46" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="H46" s="5"/>
     </row>
     <row r="47" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
@@ -1229,6 +1273,7 @@
       <c r="D47" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="H47" s="5"/>
     </row>
     <row r="48" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
@@ -1240,6 +1285,7 @@
       <c r="D48" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -1251,6 +1297,9 @@
       <c r="D49" t="s">
         <v>15</v>
       </c>
+      <c r="H49" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
@@ -1269,6 +1318,9 @@
       <c r="D52" t="s">
         <v>75</v>
       </c>
+      <c r="H52" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
@@ -1279,11 +1331,15 @@
       <c r="D54" t="s">
         <v>76</v>
       </c>
+      <c r="H54" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="55" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D55" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
@@ -1307,6 +1363,9 @@
       <c r="D59" t="s">
         <v>70</v>
       </c>
+      <c r="H59" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
@@ -1338,6 +1397,9 @@
       <c r="D64" t="s">
         <v>80</v>
       </c>
+      <c r="H64" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
@@ -1394,6 +1456,9 @@
       <c r="D71" t="s">
         <v>90</v>
       </c>
+      <c r="H71" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="L71" t="s">
         <v>129</v>
       </c>
@@ -1421,6 +1486,9 @@
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>95</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="L76" t="s">
         <v>129</v>

</xml_diff>

<commit_message>
Add SBB mock scenario
</commit_message>
<xml_diff>
--- a/mock/mock scenario variations.xlsx
+++ b/mock/mock scenario variations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\BKU\ralfrabayer\OSDM\mock\OSDM\mock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u203392\code\OSDM\mock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7834DF-EEDF-4BA3-B351-7074956E80D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3087F53F-7B24-400B-8BED-7906F568C963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{DE5B4741-31D0-4410-9DC9-14C5DAA36404}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21390" xr2:uid="{DE5B4741-31D0-4410-9DC9-14C5DAA36404}"/>
   </bookViews>
   <sheets>
     <sheet name="Features grid" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Schlapbach Andreas (IT-SCP-MVD-ETS)</author>
+  </authors>
+  <commentList>
+    <comment ref="D43" authorId="0" shapeId="0" xr:uid="{37E538FD-B4A9-4302-A1AA-7FE7F19F2F81}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Schlapbach Andreas (IT-SCP-MVD-ETS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Unsure what that is.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D44" authorId="0" shapeId="0" xr:uid="{A396B3EE-70ED-44FE-9DD7-3E42986190F0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Schlapbach Andreas (IT-SCP-MVD-ETS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Please explain?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="133">
   <si>
     <t>Shopping</t>
   </si>
@@ -115,9 +173,6 @@
   </si>
   <si>
     <t>Get travel offers</t>
-  </si>
-  <si>
-    <t>Not represented</t>
   </si>
   <si>
     <t>with optional ancillaries</t>
@@ -331,9 +386,6 @@
     <t>insufficient information in booking</t>
   </si>
   <si>
-    <t>Basel SBB - Klosters Platz</t>
-  </si>
-  <si>
     <t>SBB</t>
   </si>
   <si>
@@ -431,19 +483,41 @@
   </si>
   <si>
     <t>? - if no one else does this.</t>
+  </si>
+  <si>
+    <t>Zürich - Buchs</t>
+  </si>
+  <si>
+    <t>Basel SBB - Brig</t>
+  </si>
+  <si>
+    <t>x (one day pass)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -478,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -489,6 +563,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -504,6 +590,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -802,14 +892,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D972A9-C9B8-47DC-8286-D5354F5EB344}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D972A9-C9B8-47DC-8286-D5354F5EB344}">
   <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,9 +907,9 @@
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.85546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="56.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -833,40 +923,41 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" t="s">
         <v>100</v>
       </c>
-      <c r="F1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="I1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N1" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" t="s">
         <v>116</v>
       </c>
-      <c r="O1" t="s">
-        <v>118</v>
-      </c>
       <c r="P1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -882,41 +973,41 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>98</v>
+      <c r="E2" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N2" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" t="s">
         <v>117</v>
       </c>
-      <c r="O2" t="s">
-        <v>119</v>
-      </c>
       <c r="P2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -930,7 +1021,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -941,7 +1032,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -952,7 +1043,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -963,7 +1054,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -980,540 +1071,662 @@
         <v>14</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>24</v>
       </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
       <c r="H8" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>52</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>55</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>53</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
       <c r="H11" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>54</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
       <c r="H12" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>25</v>
       </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="H13" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>16</v>
       </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>17</v>
       </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
       <c r="H15" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>18</v>
       </c>
+      <c r="E16" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>124</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>125</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>19</v>
       </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
       <c r="L20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>26</v>
       </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
       <c r="H21" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>20</v>
       </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
       <c r="H22" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>21</v>
       </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>22</v>
       </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>23</v>
       </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>40</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>41</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
       <c r="H27" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>42</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
       <c r="L29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>45</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>120</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
       <c r="H32" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" t="s">
         <v>30</v>
       </c>
-      <c r="C35" t="s">
-        <v>35</v>
-      </c>
-      <c r="D35" t="s">
-        <v>31</v>
-      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>32</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
       <c r="L36" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>62</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
     </row>
     <row r="40" spans="2:12" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D42" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F42" s="9"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D43" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D44" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="D48" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" t="s">
         <v>63</v>
-      </c>
-      <c r="B49" t="s">
-        <v>64</v>
       </c>
       <c r="D49" t="s">
         <v>15</v>
       </c>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="H49" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>65</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="E51" s="6"/>
       <c r="L51" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>75</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E52" s="6"/>
       <c r="H52" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>78</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E53" s="6"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>76</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E54" s="6"/>
       <c r="H54" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D55" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" t="s">
         <v>66</v>
-      </c>
-      <c r="D56" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L60" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" t="s">
         <v>79</v>
       </c>
-      <c r="D64" t="s">
-        <v>80</v>
-      </c>
       <c r="H64" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L66" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>81</v>
+      </c>
+      <c r="D67" t="s">
         <v>82</v>
-      </c>
-      <c r="D67" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D70" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>87</v>
+      </c>
+      <c r="B71" t="s">
         <v>88</v>
       </c>
-      <c r="B71" t="s">
+      <c r="D71" t="s">
         <v>89</v>
       </c>
-      <c r="D71" t="s">
-        <v>90</v>
-      </c>
       <c r="H71" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L71" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L76" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
+        <v>95</v>
+      </c>
+      <c r="D77" t="s">
         <v>96</v>
-      </c>
-      <c r="D77" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>